<commit_message>
TV0002 - "ADDING STRUCTURE"
</commit_message>
<xml_diff>
--- a/db_structure.xlsx
+++ b/db_structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Утилиты\Pytnon\NEW_GIT_LIFE\teleword\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CC585B-2540-4533-9EFB-D2586850FE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6C1AE0-10CA-4018-A866-400424E8B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -384,56 +385,56 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,21 +739,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="7"/>
+      <c r="I1" s="22"/>
     </row>
     <row r="2" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -761,49 +762,49 @@
       <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="17" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="7"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="18" t="s">
         <v>24</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -811,25 +812,25 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
@@ -837,19 +838,19 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -857,19 +858,19 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L6" s="4" t="s">
@@ -877,13 +878,13 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="4" t="s">
@@ -891,18 +892,18 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="21" t="s">
+      <c r="E8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="23" t="s">
+      <c r="E9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="21" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>